<commit_message>
WORKING COPY Have caught up to previous stage but have not implemented ProjectManageMenu yet Need help with javadocs haha but tbh i can gpt it
</commit_message>
<xml_diff>
--- a/data/ProjectList.xlsx
+++ b/data/ProjectList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\LF work\LF running courses\CX2002\Assignment\2024S2\data_v1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyeyo\SC2002-Group-Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021DB320-1F74-47EA-8228-03A02A2055DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4A693A-81CC-4934-9EB0-62070F6722E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Project Name</t>
   </si>
@@ -82,6 +82,18 @@
   </si>
   <si>
     <t>Daniel,Emily</t>
+  </si>
+  <si>
+    <t>Beta Breeze</t>
+  </si>
+  <si>
+    <t>Sembahwang</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>David</t>
   </si>
 </sst>
 </file>
@@ -400,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -496,6 +508,47 @@
         <v>18</v>
       </c>
     </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>300000</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>400000</v>
+      </c>
+      <c r="I3" s="1">
+        <v>45703</v>
+      </c>
+      <c r="J3" s="1">
+        <v>45736</v>
+      </c>
+      <c r="K3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3">
+        <v>4</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
set data closeDate to 2026
</commit_message>
<xml_diff>
--- a/data/ProjectList.xlsx
+++ b/data/ProjectList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyeyo\SC2002-Group-Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4A693A-81CC-4934-9EB0-62070F6722E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD70DCF-A504-4422-B62E-A4EAB44B50B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -415,13 +415,14 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="9" max="10" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.5546875" customWidth="1"/>
     <col min="13" max="13" width="29.6640625" customWidth="1"/>
   </cols>
@@ -496,7 +497,7 @@
         <v>45703</v>
       </c>
       <c r="J2" s="1">
-        <v>45736</v>
+        <v>46101</v>
       </c>
       <c r="K2" t="s">
         <v>17</v>
@@ -537,7 +538,7 @@
         <v>45703</v>
       </c>
       <c r="J3" s="1">
-        <v>45736</v>
+        <v>46101</v>
       </c>
       <c r="K3" t="s">
         <v>21</v>

</xml_diff>